<commit_message>
Add TZA data and use a try when getting underlying data
</commit_message>
<xml_diff>
--- a/data/trading data.xlsx
+++ b/data/trading data.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="20160928 UNG" sheetId="1" r:id="rId1"/>
+    <sheet name="20160928 TZA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_20160928_UNG" localSheetId="0">'20160928 UNG'!$A$1:$B$30</definedName>
+    <definedName name="_20160928_UNG" localSheetId="0">'20160928 TZA'!$A$1:$B$30</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -19,7 +19,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="20160928 UNG" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="E:\Datos\jupyter notebooks\trading\20160928 UNG.csv" decimal="," thousands="." semicolon="1">
+    <textPr codePage="437" sourceFile="E:\Datos\jupyter notebooks\trading\data\20160928 TZA.csv" decimal="," thousands="." semicolon="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -128,18 +128,6 @@
     <t>entry_date_write_SS</t>
   </si>
   <si>
-    <t>20160928 +UNG-161021P8.00</t>
-  </si>
-  <si>
-    <t>put</t>
-  </si>
-  <si>
-    <t>UNG</t>
-  </si>
-  <si>
-    <t>20160928 +UNG-161021P9.00</t>
-  </si>
-  <si>
     <t>option_path_buy_exit</t>
   </si>
   <si>
@@ -164,9 +152,6 @@
     <t>option_buy_exit</t>
   </si>
   <si>
-    <t>20160930 +UNG-161021P8.00</t>
-  </si>
-  <si>
     <t>exit_date_buy_yy</t>
   </si>
   <si>
@@ -209,10 +194,25 @@
     <t>exit_date_write_SS</t>
   </si>
   <si>
-    <t>20160930 +UNG-161021P9.00</t>
-  </si>
-  <si>
     <t>historical_volatility_write_exit</t>
+  </si>
+  <si>
+    <t>20160928 +TZA-161021C27.00</t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>TZA</t>
+  </si>
+  <si>
+    <t>20160928 +TZA-161021C26.00</t>
+  </si>
+  <si>
+    <t>20160930 +TZA-161021C27.00</t>
+  </si>
+  <si>
+    <t>20160930 +TZA-161021C26.00</t>
   </si>
 </sst>
 </file>
@@ -584,14 +584,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="81.140625" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" customWidth="1"/>
     <col min="4" max="29" width="15.7109375" customWidth="1"/>
   </cols>
@@ -611,7 +611,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -635,7 +635,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -671,7 +671,7 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0.13</v>
+        <v>1.19</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -680,7 +680,7 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>8.5150000000000006</v>
+        <v>26.885000000000002</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -716,7 +716,7 @@
         <v>26</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -725,7 +725,7 @@
         <v>27</v>
       </c>
       <c r="B15">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -734,7 +734,7 @@
         <v>28</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -743,7 +743,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -751,7 +751,7 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <v>0.3085</v>
+        <v>0.50970000000000004</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -759,7 +759,7 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -775,7 +775,7 @@
         <v>16</v>
       </c>
       <c r="B21">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -783,7 +783,7 @@
         <v>17</v>
       </c>
       <c r="B22">
-        <v>-0.65</v>
+        <v>-1.84</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -791,7 +791,7 @@
         <v>18</v>
       </c>
       <c r="B23">
-        <v>8.4649999999999999</v>
+        <v>27.19</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -823,7 +823,7 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -831,7 +831,7 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -839,7 +839,7 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -847,44 +847,41 @@
         <v>21</v>
       </c>
       <c r="B30">
-        <v>0.3085</v>
+        <v>0.50970000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B33">
-        <v>0.14000000000000001</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34">
-        <v>8.3550000000000004</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B35">
         <v>2016</v>
@@ -892,7 +889,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B36">
         <v>9</v>
@@ -900,7 +897,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <v>30</v>
@@ -908,7 +905,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B38">
         <v>11</v>
@@ -916,63 +913,60 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B40">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B41">
-        <v>0.30620000000000003</v>
+        <v>0.53129999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B44">
-        <v>0.74</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>41</v>
-      </c>
-      <c r="B45">
-        <v>8.32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B46">
         <v>2016</v>
@@ -980,7 +974,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B47">
         <v>9</v>
@@ -988,7 +982,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <v>30</v>
@@ -996,34 +990,34 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B49">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B50">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B51">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B52">
-        <v>0.30620000000000003</v>
+        <v>0.53129999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix TZA data and finalize it
</commit_message>
<xml_diff>
--- a/data/trading data.xlsx
+++ b/data/trading data.xlsx
@@ -585,7 +585,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,6 +878,9 @@
       <c r="A34" t="s">
         <v>34</v>
       </c>
+      <c r="B34">
+        <v>26.97</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -962,6 +965,9 @@
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>37</v>
+      </c>
+      <c r="B45">
+        <v>27.02</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add intermediate results and finalize SQQQ
</commit_message>
<xml_diff>
--- a/data/trading data.xlsx
+++ b/data/trading data.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="20160928 UNG" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="E:\Datos\jupyter notebooks\trading\data\20160928 TZA.csv" decimal="," thousands="." semicolon="1">
+    <textPr codePage="437" sourceFile="E:\Datos\jupyter notebooks\trading\data\20160928 SQQQ.csv" decimal="," thousands="." semicolon="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>option_buy</t>
   </si>
@@ -146,9 +146,6 @@
     <t>underlying_write_exit</t>
   </si>
   <si>
-    <t>E:\\Datos\\bolsa\\cuenta personal\\analisis de valores\\Trades activos\\Scanning\\20160930</t>
-  </si>
-  <si>
     <t>option_buy_exit</t>
   </si>
   <si>
@@ -197,22 +194,13 @@
     <t>historical_volatility_write_exit</t>
   </si>
   <si>
-    <t>20160928 +TZA-161021C27.00</t>
-  </si>
-  <si>
     <t>call</t>
   </si>
   <si>
-    <t>TZA</t>
-  </si>
-  <si>
-    <t>20160928 +TZA-161021C26.00</t>
-  </si>
-  <si>
-    <t>20160930 +TZA-161021C27.00</t>
-  </si>
-  <si>
-    <t>20160930 +TZA-161021C26.00</t>
+    <t>20160928 +SQQQ-161021C13.00</t>
+  </si>
+  <si>
+    <t>SQQQ</t>
   </si>
 </sst>
 </file>
@@ -584,8 +572,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +615,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -635,7 +623,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -671,7 +659,7 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>1.19</v>
+        <v>0.85</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -680,7 +668,7 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>26.885000000000002</v>
+        <v>13.45</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -716,7 +704,7 @@
         <v>26</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -725,7 +713,7 @@
         <v>27</v>
       </c>
       <c r="B15">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -734,7 +722,7 @@
         <v>28</v>
       </c>
       <c r="B16">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -743,7 +731,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -751,279 +739,177 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <v>0.50970000000000004</v>
+        <v>0.43140000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B20" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
-      <c r="B21">
-        <v>26</v>
-      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="B22">
-        <v>-1.84</v>
-      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="B23">
-        <v>27.19</v>
-      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B24">
-        <v>2016</v>
-      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
-      <c r="B25">
-        <v>9</v>
-      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>28</v>
-      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B27">
-        <v>10</v>
-      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B28">
-        <v>38</v>
-      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B29">
-        <v>33</v>
-      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
-      <c r="B30">
-        <v>0.50970000000000004</v>
-      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="B33">
-        <v>1.17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="B34">
-        <v>26.97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>40</v>
       </c>
-      <c r="B35">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>41</v>
       </c>
-      <c r="B36">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>42</v>
       </c>
-      <c r="B37">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>43</v>
       </c>
-      <c r="B38">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>44</v>
       </c>
-      <c r="B39">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>45</v>
       </c>
-      <c r="B40">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41">
-        <v>0.53129999999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>35</v>
       </c>
-      <c r="B43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>36</v>
       </c>
-      <c r="B44">
-        <v>1.69</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>37</v>
       </c>
-      <c r="B45">
-        <v>27.02</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>48</v>
       </c>
-      <c r="B46">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>49</v>
       </c>
-      <c r="B47">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>50</v>
       </c>
-      <c r="B48">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>51</v>
       </c>
-      <c r="B49">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>52</v>
       </c>
-      <c r="B50">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>53</v>
-      </c>
-      <c r="B51">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52">
-        <v>0.53129999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add try for IV calculations and finalize SPY
</commit_message>
<xml_diff>
--- a/data/trading data.xlsx
+++ b/data/trading data.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="20160928 TZA" sheetId="1" r:id="rId1"/>
+    <sheet name="20160928 SQQQ" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_20160928_UNG" localSheetId="0">'20160928 TZA'!$A$1:$B$30</definedName>
+    <definedName name="_20160928_UNG" localSheetId="0">'20160928 SQQQ'!$A$1:$B$30</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -19,7 +19,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="20160928 UNG" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="E:\Datos\jupyter notebooks\trading\data\20160928 SQQQ.csv" decimal="," thousands="." semicolon="1">
+    <textPr codePage="437" sourceFile="E:\Datos\jupyter notebooks\trading\data\20160928 MBB.csv" decimal="," thousands="." semicolon="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -38,9 +38,6 @@
     <t>option_path_buy</t>
   </si>
   <si>
-    <t>E:\\Datos\\bolsa\\cuenta personal\\analisis de valores\\Trades activos\\Scanning\\20160928\\20160928</t>
-  </si>
-  <si>
     <t>option_type</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
     <t>entry_date_write_SS</t>
   </si>
   <si>
+    <t>put</t>
+  </si>
+  <si>
     <t>option_path_buy_exit</t>
   </si>
   <si>
@@ -146,6 +146,9 @@
     <t>underlying_write_exit</t>
   </si>
   <si>
+    <t>E:\\Datos\\bolsa\\cuenta personal\\analisis de valores\\Trades activos\\Scanning\\20160930</t>
+  </si>
+  <si>
     <t>option_buy_exit</t>
   </si>
   <si>
@@ -194,13 +197,10 @@
     <t>historical_volatility_write_exit</t>
   </si>
   <si>
-    <t>call</t>
-  </si>
-  <si>
-    <t>20160928 +SQQQ-161021C13.00</t>
-  </si>
-  <si>
-    <t>SQQQ</t>
+    <t>20160930 +SPY-161021P216.00</t>
+  </si>
+  <si>
+    <t>SPY</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,10 +586,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -607,29 +607,29 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>216</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>2016</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>21</v>
@@ -656,25 +656,25 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>0.85</v>
+        <v>2.66</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>13.45</v>
+        <v>215.63499999999999</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>2016</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>9</v>
@@ -692,43 +692,43 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
         <v>56</v>
@@ -736,75 +736,75 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18">
-        <v>0.43140000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -824,42 +824,42 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
@@ -879,37 +879,37 @@
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eliminate empty data in bid and ask lists and finalize OIH
</commit_message>
<xml_diff>
--- a/data/trading data.xlsx
+++ b/data/trading data.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="20160928 SQQQ" sheetId="1" r:id="rId1"/>
+    <sheet name="20160930 OIH" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_20160928_UNG" localSheetId="0">'20160928 SQQQ'!$A$1:$B$30</definedName>
+    <definedName name="_20160928_UNG" localSheetId="0">'20160930 OIH'!$A$1:$B$30</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>option_buy</t>
   </si>
@@ -125,9 +125,6 @@
     <t>entry_date_write_SS</t>
   </si>
   <si>
-    <t>put</t>
-  </si>
-  <si>
     <t>option_path_buy_exit</t>
   </si>
   <si>
@@ -197,10 +194,16 @@
     <t>historical_volatility_write_exit</t>
   </si>
   <si>
-    <t>20160930 +SPY-161021P216.00</t>
-  </si>
-  <si>
-    <t>SPY</t>
+    <t>call</t>
+  </si>
+  <si>
+    <t>20160930 +OIH-161021C30.00</t>
+  </si>
+  <si>
+    <t>20160930 +OIH-161021C29.00</t>
+  </si>
+  <si>
+    <t>OIH</t>
   </si>
 </sst>
 </file>
@@ -573,7 +576,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -615,7 +618,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -623,7 +626,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>216</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -659,7 +662,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>2.66</v>
+        <v>0.42</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -668,7 +671,7 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>215.63499999999999</v>
+        <v>29.05</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -722,7 +725,7 @@
         <v>27</v>
       </c>
       <c r="B16">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -731,7 +734,7 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -739,177 +742,213 @@
         <v>7</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>0.37669999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
+      <c r="B21">
+        <v>29</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
+      <c r="B22">
+        <v>-0.86</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
+      <c r="B23">
+        <v>29.035</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
+      <c r="B24">
+        <v>2016</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
+      <c r="B26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
+      <c r="B28">
+        <v>24</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
+      <c r="B30">
+        <v>0.37669999999999998</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove lines of options with header data and add new trades
</commit_message>
<xml_diff>
--- a/data/trading data.xlsx
+++ b/data/trading data.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="20160930 HYG" sheetId="1" r:id="rId1"/>
+    <sheet name="20160930 SQQQ" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_20160928_UNG" localSheetId="0">'20160930 HYG'!$A$1:$B$30</definedName>
+    <definedName name="_20160928_UNG" localSheetId="0">'20160930 SQQQ'!$A$1:$B$30</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>

</xml_diff>

<commit_message>
Add FXI data and minor modifications
</commit_message>
<xml_diff>
--- a/data/trading data.xlsx
+++ b/data/trading data.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="20161004 SPY" sheetId="1" r:id="rId1"/>
+    <sheet name="20161004 FXI" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_20160928_UNG" localSheetId="0">'20161004 SPY'!$A$1:$D$52</definedName>
+    <definedName name="_20160928_UNG" localSheetId="0">'20161004 FXI'!$A$1:$D$52</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -194,16 +194,16 @@
     <t>put</t>
   </si>
   <si>
-    <t>SPY</t>
-  </si>
-  <si>
-    <t>20161004 +SPY-161021P216.00</t>
-  </si>
-  <si>
     <t>E:\\Datos\\bolsa\\cuenta personal\\analisis de valores\\Trades activos\\Scanning\\20161004</t>
   </si>
   <si>
-    <t>20161004 +SPY-161021P217.00</t>
+    <t>20161004 +FXI-161021P38.00</t>
+  </si>
+  <si>
+    <t>FXI</t>
+  </si>
+  <si>
+    <t>20161004 +FXI-161021P37.00</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
   <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -610,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -626,7 +626,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>216</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -662,7 +662,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>2.17</v>
+        <v>0.26</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -671,7 +671,7 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>215.9</v>
+        <v>38.17</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -716,7 +716,7 @@
         <v>26</v>
       </c>
       <c r="B15">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -725,7 +725,7 @@
         <v>27</v>
       </c>
       <c r="B16">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2"/>
     </row>
@@ -734,7 +734,7 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
         <v>7</v>
       </c>
       <c r="B18">
-        <v>0.14169999999999999</v>
+        <v>0.2162</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -750,7 +750,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -758,7 +758,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -766,7 +766,7 @@
         <v>15</v>
       </c>
       <c r="B21">
-        <v>217</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -774,7 +774,7 @@
         <v>16</v>
       </c>
       <c r="B22">
-        <v>-2.6</v>
+        <v>-0.54</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>17</v>
       </c>
       <c r="B23">
-        <v>215.97</v>
+        <v>38.215000000000003</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -830,7 +830,7 @@
         <v>30</v>
       </c>
       <c r="B29">
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>20</v>
       </c>
       <c r="B30">
-        <v>0.14169999999999999</v>
+        <v>0.2162</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>